<commit_message>
I made some changes to the documents
</commit_message>
<xml_diff>
--- a/docs/EchoPlay_Materialliste_250514.xlsx
+++ b/docs/EchoPlay_Materialliste_250514.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomni\Documents\Schule-lokal\IMS\IP\ims.project.echoplay\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A695FB57-B065-48CD-B4E0-899A48193AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5272450-9B18-4957-9DF3-8C090738724F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-130" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Komponente</t>
   </si>
@@ -144,6 +144,36 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>SparkFun Carrier Board</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/sparkfun-electronics/16885/13282886?s=N4IgTCBcDaICIFEBqBaAjANgBxYKwgF0BfIA</t>
+  </si>
+  <si>
+    <t>1568-16885-ND</t>
+  </si>
+  <si>
+    <t>DEV-16885</t>
+  </si>
+  <si>
+    <t>SparkFun ESP32 Processor</t>
+  </si>
+  <si>
+    <t>WRL-16781</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/sparkfun-electronics/16781/13282892?s=N4IgTCBcDaIOoCUAyBaAjANgOwA40gF0BfIA</t>
+  </si>
+  <si>
+    <t>1568-16781-ND</t>
+  </si>
+  <si>
+    <t>Carrier Board um den ESP32 Prozessor zu halten</t>
+  </si>
+  <si>
+    <t>ESP32 Prozessor um alles zu rechnen</t>
   </si>
 </sst>
 </file>
@@ -512,27 +542,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="53.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -561,7 +591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -590,7 +620,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -619,7 +649,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -648,7 +678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -677,7 +707,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -706,22 +736,80 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="H7" s="5">
-        <f>SUM(H2:H6)</f>
-        <v>22.64</v>
-      </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H8" s="1"/>
+        <v>20.5</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="5">
+        <v>20.6</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="5">
+        <f>SUM(H2:H8)</f>
+        <v>63.74</v>
+      </c>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H10" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Ich habe mein Repository einbisschen auferäumt
</commit_message>
<xml_diff>
--- a/docs/EchoPlay_Materialliste_250514.xlsx
+++ b/docs/EchoPlay_Materialliste_250514.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomni\Documents\Schule-lokal\IMS\IP\ims.project.echoplay\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5272450-9B18-4957-9DF3-8C090738724F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06D61AB-BF14-4DF6-A8A6-C6DC01406F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-130" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -250,13 +250,14 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -542,27 +543,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="53.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -591,7 +592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -620,7 +621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -649,7 +650,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -678,7 +679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -707,7 +708,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -736,7 +737,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -765,7 +766,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -794,7 +795,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -808,8 +809,11 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G11" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -818,9 +822,11 @@
     <hyperlink ref="G4" r:id="rId3" xr:uid="{EC91A0BE-2C88-465A-8E1D-A114EFEF34DD}"/>
     <hyperlink ref="G3" r:id="rId4" xr:uid="{5479E7E6-6EC2-403C-B13F-ADB612287F3D}"/>
     <hyperlink ref="G2" r:id="rId5" xr:uid="{DB8498AC-4527-481C-994A-4B94A89D836E}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{2EB9479A-6473-4858-A1E0-72FD71C933E8}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{9C93F839-7F96-41F3-90A2-58A19CE9D4B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="81" fitToHeight="0" orientation="landscape" r:id="rId6"/>
+  <pageSetup paperSize="9" scale="81" fitToHeight="0" orientation="landscape" r:id="rId8"/>
   <headerFooter>
     <oddHeader>&amp;LMaterialliste 
 &amp;CEchoPlay&amp;R&amp;D</oddHeader>

</xml_diff>